<commit_message>
Get IMACLIM World region out of aggregation table
</commit_message>
<xml_diff>
--- a/data/IMACLIM_equivalent/IMACLIM_format_equivalent.xlsx
+++ b/data/IMACLIM_equivalent/IMACLIM_format_equivalent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mpotfer\Stage\MatMat-Trade\data\IMACLIM_equivalent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294B8DA1-1D40-4E8E-B5A7-4C6AFF5C1639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569EE9F9-33B3-483F-8C57-5B563516636F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>AFR</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>World</t>
   </si>
   <si>
     <t>Agriculture</t>
@@ -138,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -174,11 +171,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -187,6 +197,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -493,11 +510,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="14" max="14" width="8.88671875" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -533,12 +551,10 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -580,9 +596,6 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -622,9 +635,6 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
         <v>0</v>
       </c>
     </row>
@@ -668,9 +678,6 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -712,9 +719,6 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -756,9 +760,6 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -800,9 +801,6 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -844,9 +842,6 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -888,9 +883,6 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -932,9 +924,6 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -976,9 +965,6 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1020,12 +1006,9 @@
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1064,53 +1047,9 @@
       <c r="M13">
         <v>1</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="14" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1132,45 +1071,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1211,7 +1150,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1252,7 +1191,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1293,7 +1232,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1334,7 +1273,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1375,7 +1314,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1416,7 +1355,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1457,7 +1396,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1498,7 +1437,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1539,7 +1478,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1580,7 +1519,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1621,7 +1560,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>